<commit_message>
Atualização automática de IVOTI.xlsx
</commit_message>
<xml_diff>
--- a/IVOTI.xlsx
+++ b/IVOTI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9955660A-E6B1-48F7-A150-80E03D3A8C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{78365B54-6E16-482C-A855-8A7CE66FCD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -999,7 +999,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1059,36 +1059,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1122,14 +1098,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1147,7 +1119,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1162,7 +1133,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{4DF206FE-35DF-4675-B1DE-3EB63AB78C9D}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{05B4B010-2026-4E76-9200-DB7CB8D788AF}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1192,10 +1163,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DE6E5F8-A435-4612-8641-220E4CAA6D21}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B91827B7-3A5B-4D99-B3C8-275CBECB4201}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1233,7 +1204,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{880FA078-8AE6-4B92-BC66-8B0FB73854EE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61923272-4548-4897-AA74-58BE78CCF16E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1296,7 +1267,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F90B42DE-5335-4A0F-A9C4-D9D992C7E5E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFB1478B-2491-455B-82B1-61CA504CE4E3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1315,7 +1286,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{464CF4F7-EC58-C6B2-DE0C-F68B61D026F0}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47BA202F-1233-C9D6-807E-3B8D63C696A7}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1364,7 +1335,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1050556-63DA-1BDA-5831-3C33A8756872}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D188C656-4ABA-BF41-85BF-9FD159AB6986}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1383,7 +1354,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1B99C2C-A418-5149-CC38-8FB6A7B2A8D8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2579F8B-1A43-7662-1FDF-002E8C2907E4}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1414,7 +1385,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D151534A-7769-CE8F-1DD2-4F00C9F912E8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{489E649C-6115-58C7-DB3B-5E4A6C172D4F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1445,7 +1416,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BDAD6A3-B91A-85E3-BF53-915C7271C341}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C5B24B3-0F94-8494-C720-DA87412078A1}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1488,7 +1459,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DAD9ABE-1C7D-4D21-BFFF-00CAC39E2FFC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{123E8329-7677-4C95-88BC-858FB1843771}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1526,7 +1497,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65D8A832-8897-4094-8B94-2453D137CE5F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5F8EA8B-F1AB-4513-AB5C-1C494C728B45}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1569,7 +1540,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6539D88-8612-4768-9BED-0F983F6E87FA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{417225D5-EDD8-4451-A81D-A3F6C4EDE160}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1882,7 +1853,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{217DE5E5-075C-4D27-9CC7-12C391C1064D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA65D671-9059-4CE0-BCB7-0F01EBA4DE18}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1894,98 +1865,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="31"/>
-    <col min="6" max="6" width="2" style="31" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="31" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="31"/>
+    <col min="1" max="5" width="12.5703125" style="28"/>
+    <col min="6" max="6" width="2" style="28" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="28" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="30"/>
+      <c r="F1" s="27"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="30"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="30"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="30"/>
+      <c r="F4" s="27"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="30"/>
+      <c r="F5" s="27"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="30"/>
+      <c r="F6" s="27"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="30"/>
+      <c r="F7" s="27"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="30"/>
+      <c r="F8" s="27"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="30"/>
+      <c r="F9" s="27"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="30"/>
+      <c r="F10" s="27"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="30"/>
+      <c r="F11" s="27"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="30"/>
+      <c r="F12" s="27"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="30"/>
+      <c r="F13" s="27"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="30"/>
+      <c r="F14" s="27"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="30"/>
+      <c r="F15" s="27"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="30"/>
+      <c r="F16" s="27"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="30"/>
+      <c r="F17" s="27"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="30"/>
+      <c r="F18" s="27"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="30"/>
+      <c r="F19" s="27"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="30"/>
+      <c r="F20" s="27"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="30"/>
+      <c r="F21" s="27"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="30"/>
+      <c r="F22" s="27"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="30"/>
+      <c r="F23" s="27"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="30"/>
+      <c r="F24" s="27"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="30"/>
+      <c r="F25" s="27"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="30"/>
+      <c r="F26" s="27"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="30"/>
+      <c r="F27" s="27"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="30"/>
+      <c r="F28" s="27"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="30"/>
+      <c r="F29" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5132,19 +5103,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>256</v>
       </c>
     </row>
@@ -5167,46 +5138,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="18" t="s">
         <v>259</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="17" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="17" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="17" t="s">
         <v>260</v>
       </c>
     </row>
@@ -5231,99 +5202,100 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>264</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>266</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="20" t="s">
         <v>267</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="21" t="s">
         <v>269</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="19" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="22">
         <v>45839</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="23" t="s">
         <v>279</v>
       </c>
-      <c r="F2" s="27">
+      <c r="F2" s="24">
         <v>4140</v>
       </c>
-      <c r="G2" s="27">
+      <c r="G2" s="24">
         <v>852</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="M2" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="O2" s="26" t="s">
         <v>282</v>
       </c>
     </row>

</xml_diff>